<commit_message>
interaction update + statistics
</commit_message>
<xml_diff>
--- a/3 TP Analysis/01 - Data/PROCESSED_benthic_cover_March_2021.xlsx
+++ b/3 TP Analysis/01 - Data/PROCESSED_benthic_cover_March_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shannon/GitHub/NFI_benthic_community/3 TP Analysis/01 - Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B47AA08-D213-4348-97B4-23BC3DC77AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66B9B5B-6D94-8544-88EA-B8FC240698CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="680" windowWidth="26720" windowHeight="15900" xr2:uid="{C9E9F2B5-9E51-DB46-924D-72FA6A54096A}"/>
+    <workbookView xWindow="7180" yWindow="1080" windowWidth="26720" windowHeight="15900" xr2:uid="{C9E9F2B5-9E51-DB46-924D-72FA6A54096A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1432,7 +1432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1451,6 +1451,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD9EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1464,10 +1470,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1784,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80E967E-8A63-DD4E-8DF1-D50E3DB1E9FD}">
   <dimension ref="A1:AE431"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A390" workbookViewId="0">
+      <selection activeCell="V429" sqref="V429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42358,98 +42365,98 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A428" s="2" t="s">
+    <row r="428" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A428" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B428">
-        <v>0</v>
-      </c>
-      <c r="C428">
-        <v>0</v>
-      </c>
-      <c r="D428">
-        <v>0</v>
-      </c>
-      <c r="E428">
-        <v>0</v>
-      </c>
-      <c r="F428">
-        <v>1</v>
-      </c>
-      <c r="G428">
-        <v>0</v>
-      </c>
-      <c r="H428">
-        <v>0</v>
-      </c>
-      <c r="I428">
+      <c r="B428" s="3">
+        <v>0</v>
+      </c>
+      <c r="C428" s="3">
+        <v>0</v>
+      </c>
+      <c r="D428" s="3">
+        <v>0</v>
+      </c>
+      <c r="E428" s="3">
+        <v>0</v>
+      </c>
+      <c r="F428" s="3">
+        <v>1</v>
+      </c>
+      <c r="G428" s="3">
+        <v>0</v>
+      </c>
+      <c r="H428" s="3">
+        <v>0</v>
+      </c>
+      <c r="I428" s="3">
         <v>34</v>
       </c>
-      <c r="J428">
-        <v>0</v>
-      </c>
-      <c r="K428">
-        <v>0</v>
-      </c>
-      <c r="L428">
+      <c r="J428" s="3">
+        <v>0</v>
+      </c>
+      <c r="K428" s="3">
+        <v>0</v>
+      </c>
+      <c r="L428" s="3">
+        <v>0</v>
+      </c>
+      <c r="M428" s="3">
+        <v>0</v>
+      </c>
+      <c r="N428" s="3">
+        <v>0</v>
+      </c>
+      <c r="O428" s="3">
+        <v>0</v>
+      </c>
+      <c r="P428" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q428" s="3">
+        <v>19</v>
+      </c>
+      <c r="R428" s="3">
+        <v>0</v>
+      </c>
+      <c r="S428" s="3">
+        <v>0</v>
+      </c>
+      <c r="T428" s="3">
+        <v>0</v>
+      </c>
+      <c r="U428" s="3">
+        <v>0</v>
+      </c>
+      <c r="V428" s="3">
+        <v>5</v>
+      </c>
+      <c r="W428" s="3">
+        <v>24</v>
+      </c>
+      <c r="X428" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y428" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z428" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA428" s="3">
         <v>2</v>
       </c>
-      <c r="M428">
-        <v>0</v>
-      </c>
-      <c r="N428">
-        <v>0</v>
-      </c>
-      <c r="O428">
-        <v>0</v>
-      </c>
-      <c r="P428">
-        <v>0</v>
-      </c>
-      <c r="Q428">
-        <v>19</v>
-      </c>
-      <c r="R428">
-        <v>0</v>
-      </c>
-      <c r="S428">
-        <v>0</v>
-      </c>
-      <c r="T428">
-        <v>0</v>
-      </c>
-      <c r="U428">
-        <v>0</v>
-      </c>
-      <c r="V428">
-        <v>3</v>
-      </c>
-      <c r="W428">
-        <v>24</v>
-      </c>
-      <c r="X428">
-        <v>10</v>
-      </c>
-      <c r="Y428">
-        <v>0</v>
-      </c>
-      <c r="Z428">
-        <v>1</v>
-      </c>
-      <c r="AA428">
+      <c r="AB428" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC428" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD428" s="3">
         <v>2</v>
       </c>
-      <c r="AB428">
-        <v>0</v>
-      </c>
-      <c r="AC428">
-        <v>0</v>
-      </c>
-      <c r="AD428">
-        <v>2</v>
-      </c>
-      <c r="AE428">
+      <c r="AE428" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>